<commit_message>
minor change excel sheet
</commit_message>
<xml_diff>
--- a/methods-excel.xlsx
+++ b/methods-excel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\OneDrive\Desktop\Git\Thesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\sciebo\Neu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C11DE390-54E9-4396-84DD-7C09DC50417B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D5C607-30FC-4192-A370-9FCD0800B0B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{30D774E5-5D97-4036-9EF5-DFCDE9589F87}"/>
   </bookViews>
@@ -2672,8 +2672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A03FB77-42A8-4496-B47B-A02E1CA4B62A}">
   <dimension ref="A1:N199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B84" workbookViewId="0">
-      <selection activeCell="D89" sqref="D89"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>